<commit_message>
Verificar dados de data e preço
</commit_message>
<xml_diff>
--- a/bd/Modelo Lógico.xlsx
+++ b/bd/Modelo Lógico.xlsx
@@ -1,30 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FIC\Desktop\Projeto\bd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luana e Regis\Desktop\CZBook\Senai_CZBook\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C9FA71-BB75-4534-B2F8-E6AC60CA959A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-20610" yWindow="2280" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="61">
   <si>
     <t>TiposUsuários</t>
   </si>
@@ -204,12 +210,15 @@
   </si>
   <si>
     <t>cobre=29</t>
+  </si>
+  <si>
+    <t>idUsuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
@@ -328,9 +337,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -340,35 +372,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -654,11 +666,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,7 +680,7 @@
     <col min="4" max="4" width="32.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.5703125" style="10" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125" style="7" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
@@ -676,25 +688,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="E2" s="4" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="J2" s="14" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="J2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
     </row>
     <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
@@ -703,33 +716,36 @@
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="J3" s="15" t="s">
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="J3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="K3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="M3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="P3" s="15" t="s">
+      <c r="P3" s="10" t="s">
         <v>47</v>
       </c>
     </row>
@@ -740,33 +756,36 @@
       <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="5">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="J4" s="15">
-        <v>1</v>
-      </c>
-      <c r="K4" s="15" t="s">
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="J4" s="10">
+        <v>1</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="15">
-        <v>1</v>
-      </c>
-      <c r="N4" s="15">
-        <v>1</v>
-      </c>
-      <c r="O4" s="16">
+      <c r="M4" s="10">
+        <v>1</v>
+      </c>
+      <c r="N4" s="10">
+        <v>1</v>
+      </c>
+      <c r="O4" s="11">
         <v>33559</v>
       </c>
-      <c r="P4" s="17">
+      <c r="P4" s="12">
         <v>43.99</v>
       </c>
     </row>
@@ -777,33 +796,36 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="5">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
         <v>2</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="J5" s="15">
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="J5" s="10">
         <v>2</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="M5" s="15">
-        <v>1</v>
-      </c>
-      <c r="N5" s="15">
+      <c r="M5" s="10">
+        <v>1</v>
+      </c>
+      <c r="N5" s="10">
         <v>2</v>
       </c>
-      <c r="O5" s="16">
+      <c r="O5" s="11">
         <v>43874</v>
       </c>
-      <c r="P5" s="17">
+      <c r="P5" s="12">
         <v>87.5</v>
       </c>
     </row>
@@ -814,296 +836,296 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="15">
-        <v>3</v>
-      </c>
-      <c r="K6" s="15" t="s">
+      <c r="J6" s="10">
+        <v>3</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="M6" s="15">
-        <v>1</v>
-      </c>
-      <c r="N6" s="15">
-        <v>1</v>
-      </c>
-      <c r="O6" s="16">
+      <c r="M6" s="10">
+        <v>1</v>
+      </c>
+      <c r="N6" s="10">
+        <v>1</v>
+      </c>
+      <c r="O6" s="11">
         <v>34164</v>
       </c>
-      <c r="P6" s="17">
+      <c r="P6" s="12">
         <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="J7" s="15">
+      <c r="J7" s="10">
         <v>4</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="15">
-        <v>1</v>
-      </c>
-      <c r="N7" s="15">
+      <c r="M7" s="10">
+        <v>1</v>
+      </c>
+      <c r="N7" s="10">
         <v>2</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7" s="11">
         <v>16529</v>
       </c>
-      <c r="P7" s="17">
+      <c r="P7" s="12">
         <v>78</v>
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="J8" s="15">
+      <c r="J8" s="10">
         <v>5</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="M8" s="15">
-        <v>1</v>
-      </c>
-      <c r="N8" s="15">
-        <v>3</v>
-      </c>
-      <c r="O8" s="16">
+      <c r="M8" s="10">
+        <v>1</v>
+      </c>
+      <c r="N8" s="10">
+        <v>3</v>
+      </c>
+      <c r="O8" s="11">
         <v>44133</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="12">
         <v>30.7</v>
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="19" t="str">
+      <c r="C11" s="13" t="str">
         <f>B3</f>
         <v>idTiposUsuários</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="F11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="6"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="19">
-        <v>1</v>
-      </c>
-      <c r="C12" s="19">
-        <v>1</v>
-      </c>
-      <c r="D12" s="19" t="s">
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" s="13">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="F12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="19">
+      <c r="B13" s="13">
         <v>2</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="13">
         <v>2</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="7">
-        <v>1</v>
-      </c>
-      <c r="K13" s="7" t="s">
+      <c r="J13" s="4">
+        <v>1</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="19">
-        <v>3</v>
-      </c>
-      <c r="C14" s="19">
-        <v>3</v>
-      </c>
-      <c r="D14" s="19" t="s">
+      <c r="B14" s="13">
+        <v>3</v>
+      </c>
+      <c r="C14" s="13">
+        <v>3</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="20" t="s">
+      <c r="F14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="4">
         <v>2</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="19">
+      <c r="B15" s="13">
         <v>4</v>
       </c>
-      <c r="C15" s="19">
-        <v>3</v>
-      </c>
-      <c r="D15" s="19" t="s">
+      <c r="C15" s="13">
+        <v>3</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="13">
         <v>123123</v>
       </c>
-      <c r="J15" s="7">
-        <v>3</v>
-      </c>
-      <c r="K15" s="7" t="s">
+      <c r="J15" s="4">
+        <v>3</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="21">
+      <c r="B16" s="15">
         <v>5</v>
       </c>
-      <c r="C16" s="21">
-        <v>3</v>
-      </c>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="15">
+        <v>3</v>
+      </c>
+      <c r="D16" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J16" s="4">
         <v>4</v>
       </c>
-      <c r="K16" s="7" t="s">
+      <c r="K16" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="J17" s="7">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="J17" s="4">
         <v>5</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="K17" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" s="13" t="s">
+      <c r="C23" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="13">
-        <v>1</v>
-      </c>
-      <c r="C24" s="13">
-        <v>3</v>
-      </c>
-      <c r="D24" s="13" t="s">
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
+        <v>3</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="13">
+      <c r="B25" s="9">
         <v>2</v>
       </c>
-      <c r="C25" s="13">
-        <v>3</v>
-      </c>
-      <c r="D25" s="13" t="s">
+      <c r="C25" s="9">
+        <v>3</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="13">
-        <v>3</v>
-      </c>
-      <c r="C26" s="13">
-        <v>3</v>
-      </c>
-      <c r="D26" s="13" t="s">
+      <c r="B26" s="9">
+        <v>3</v>
+      </c>
+      <c r="C26" s="9">
+        <v>3</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1111,18 +1133,18 @@
   <mergeCells count="6">
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="E2:F2"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="J2:P2"/>
+    <mergeCell ref="D2:F2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E12" r:id="rId1"/>
-    <hyperlink ref="E13" r:id="rId2"/>
-    <hyperlink ref="E14" r:id="rId3"/>
-    <hyperlink ref="F14" r:id="rId4"/>
-    <hyperlink ref="E15" r:id="rId5"/>
-    <hyperlink ref="E16" r:id="rId6"/>
+    <hyperlink ref="E12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E15" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>

</xml_diff>